<commit_message>
update Fri. brief stat
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="0" windowWidth="30660" windowHeight="17580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37580" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>result_Joyce_IR</t>
   </si>
@@ -55,6 +55,66 @@
   </si>
   <si>
     <t>result_Jennifer_List</t>
+  </si>
+  <si>
+    <t>result_Clemens_List</t>
+  </si>
+  <si>
+    <t>result_Clemens_IR</t>
+  </si>
+  <si>
+    <t>result_Mike_List</t>
+  </si>
+  <si>
+    <t>result_Mike_IR</t>
+  </si>
+  <si>
+    <t>Lisa List</t>
+  </si>
+  <si>
+    <t>Lisa IR</t>
+  </si>
+  <si>
+    <t>Bharath IR</t>
+  </si>
+  <si>
+    <t>Bharath List</t>
+  </si>
+  <si>
+    <t>Kyunam List</t>
+  </si>
+  <si>
+    <t>Kyunam IR</t>
+  </si>
+  <si>
+    <t>Peter Lists</t>
+  </si>
+  <si>
+    <t>Peter IR</t>
+  </si>
+  <si>
+    <t>Jeremy List</t>
+  </si>
+  <si>
+    <t>Jeremy IR</t>
+  </si>
+  <si>
+    <t>Anthony List</t>
+  </si>
+  <si>
+    <t>Anthony IR</t>
+  </si>
+  <si>
+    <t>Antoine List</t>
+  </si>
+  <si>
+    <t>Antoine IR</t>
+  </si>
+  <si>
+    <t>Peggy List</t>
+  </si>
+  <si>
+    <t>Peggy IR</t>
   </si>
 </sst>
 </file>
@@ -114,8 +174,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,19 +202,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -499,9 +563,13 @@
     <col min="8" max="8" width="23.1640625" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1">
+    <row r="1" spans="1:30" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -532,8 +600,68 @@
       <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:30">
       <c r="A2" s="1">
         <v>7.9614899158499997</v>
       </c>
@@ -564,8 +692,68 @@
       <c r="J2">
         <v>9.2856898307800009</v>
       </c>
+      <c r="K2">
+        <v>10.6902940273</v>
+      </c>
+      <c r="L2">
+        <v>4.1410629749299996</v>
+      </c>
+      <c r="M2">
+        <v>4.3230459689999998</v>
+      </c>
+      <c r="N2">
+        <v>4.5126390457200003</v>
+      </c>
+      <c r="O2">
+        <v>6.0633990764999997</v>
+      </c>
+      <c r="P2">
+        <v>5.1759588718399998</v>
+      </c>
+      <c r="Q2">
+        <v>8.0362579822499995</v>
+      </c>
+      <c r="R2">
+        <v>7.2060239314999999</v>
+      </c>
+      <c r="S2">
+        <v>13.3588449955</v>
+      </c>
+      <c r="T2">
+        <v>10.2383198738</v>
+      </c>
+      <c r="U2">
+        <v>9.1958041191100008</v>
+      </c>
+      <c r="V2">
+        <v>6.9320771694200003</v>
+      </c>
+      <c r="W2">
+        <v>10.963108778</v>
+      </c>
+      <c r="X2">
+        <v>7.11388397217</v>
+      </c>
+      <c r="Y2">
+        <v>6.0222041606900003</v>
+      </c>
+      <c r="Z2">
+        <v>8.5321600437199994</v>
+      </c>
+      <c r="AA2">
+        <v>10.476042032200001</v>
+      </c>
+      <c r="AB2">
+        <v>5.0028641223900001</v>
+      </c>
+      <c r="AC2">
+        <v>7.8522348403900004</v>
+      </c>
+      <c r="AD2">
+        <v>5.4676089286799998</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:30">
       <c r="A3" s="1">
         <v>4.8067808151199998</v>
       </c>
@@ -596,8 +784,65 @@
       <c r="J3">
         <v>14.849549055100001</v>
       </c>
+      <c r="K3">
+        <v>9.6922490596799999</v>
+      </c>
+      <c r="L3">
+        <v>4.0449960231800004</v>
+      </c>
+      <c r="M3">
+        <v>7.8282320499400004</v>
+      </c>
+      <c r="N3">
+        <v>7.7525489330299999</v>
+      </c>
+      <c r="O3">
+        <v>14.592661142300001</v>
+      </c>
+      <c r="Q3">
+        <v>5.8225100040399997</v>
+      </c>
+      <c r="R3">
+        <v>5.4680030345899997</v>
+      </c>
+      <c r="S3">
+        <v>9.1313791275000007</v>
+      </c>
+      <c r="T3">
+        <v>7.4002039432500002</v>
+      </c>
+      <c r="U3">
+        <v>9.0878639221200004</v>
+      </c>
+      <c r="V3">
+        <v>11.175037145599999</v>
+      </c>
+      <c r="W3">
+        <v>5.4011659622200003</v>
+      </c>
+      <c r="X3">
+        <v>4.4733150005300004</v>
+      </c>
+      <c r="Y3">
+        <v>8.9893550872799999</v>
+      </c>
+      <c r="Z3">
+        <v>5.1297099590300004</v>
+      </c>
+      <c r="AA3">
+        <v>7.7840139865899998</v>
+      </c>
+      <c r="AB3">
+        <v>4.3651661872899998</v>
+      </c>
+      <c r="AC3">
+        <v>7.7849428653699997</v>
+      </c>
+      <c r="AD3">
+        <v>8.5599918365499992</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:30">
       <c r="A4" s="1">
         <v>5.6240048408499996</v>
       </c>
@@ -626,8 +871,62 @@
       <c r="J4">
         <v>7.96130800247</v>
       </c>
+      <c r="K4">
+        <v>6.0300981998400003</v>
+      </c>
+      <c r="L4">
+        <v>5.9563770294199996</v>
+      </c>
+      <c r="M4">
+        <v>8.2111420631400005</v>
+      </c>
+      <c r="N4">
+        <v>6.3721070289600004</v>
+      </c>
+      <c r="O4">
+        <v>6.92248106003</v>
+      </c>
+      <c r="P4">
+        <v>5.4192841053</v>
+      </c>
+      <c r="Q4">
+        <v>5.3753728866600001</v>
+      </c>
+      <c r="R4">
+        <v>4.4524378776600004</v>
+      </c>
+      <c r="S4">
+        <v>6.4739739894900001</v>
+      </c>
+      <c r="T4">
+        <v>7.9443469047499997</v>
+      </c>
+      <c r="U4">
+        <v>3.9572138786300002</v>
+      </c>
+      <c r="V4">
+        <v>4.9566390514399998</v>
+      </c>
+      <c r="W4">
+        <v>12.5399329662</v>
+      </c>
+      <c r="Y4">
+        <v>7.5216917991600001</v>
+      </c>
+      <c r="AA4">
+        <v>5.3050129413600002</v>
+      </c>
+      <c r="AB4">
+        <v>10.0883159637</v>
+      </c>
+      <c r="AC4">
+        <v>4.2455191612199998</v>
+      </c>
+      <c r="AD4">
+        <v>4.1569168567699997</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:30">
       <c r="A5" s="1">
         <v>8.5992159843400007</v>
       </c>
@@ -656,8 +955,65 @@
       <c r="J5">
         <v>9.8124041557300004</v>
       </c>
+      <c r="K5">
+        <v>5.5176250934600004</v>
+      </c>
+      <c r="L5">
+        <v>4.0669529437999996</v>
+      </c>
+      <c r="M5">
+        <v>16.295876979799999</v>
+      </c>
+      <c r="N5">
+        <v>4.4166510105099999</v>
+      </c>
+      <c r="O5">
+        <v>9.0494170188900007</v>
+      </c>
+      <c r="P5">
+        <v>4.7539489269299997</v>
+      </c>
+      <c r="Q5">
+        <v>6.0068490505199996</v>
+      </c>
+      <c r="R5">
+        <v>11.6618080139</v>
+      </c>
+      <c r="S5">
+        <v>7.1607379913300004</v>
+      </c>
+      <c r="U5">
+        <v>4.4833920002000003</v>
+      </c>
+      <c r="V5">
+        <v>5.9676060676600002</v>
+      </c>
+      <c r="W5">
+        <v>4.1046979427299997</v>
+      </c>
+      <c r="X5">
+        <v>3.4359340667699998</v>
+      </c>
+      <c r="Y5">
+        <v>4.6090378761300004</v>
+      </c>
+      <c r="Z5">
+        <v>4.2276520729099998</v>
+      </c>
+      <c r="AA5">
+        <v>4.3470568656899999</v>
+      </c>
+      <c r="AB5">
+        <v>4.4491310119599996</v>
+      </c>
+      <c r="AC5">
+        <v>7.2515869140599998</v>
+      </c>
+      <c r="AD5">
+        <v>5.3877310752899996</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:30">
       <c r="A6" s="1">
         <v>4.72080397606</v>
       </c>
@@ -684,8 +1040,68 @@
       <c r="J6">
         <v>9.2350628375999992</v>
       </c>
+      <c r="K6">
+        <v>7.8136389255500003</v>
+      </c>
+      <c r="L6">
+        <v>5.19321894646</v>
+      </c>
+      <c r="M6">
+        <v>9.8995192050899998</v>
+      </c>
+      <c r="N6">
+        <v>4.7640841007199999</v>
+      </c>
+      <c r="O6">
+        <v>9.6020271778099993</v>
+      </c>
+      <c r="P6">
+        <v>6.36286091805</v>
+      </c>
+      <c r="Q6">
+        <v>6.9859220981599996</v>
+      </c>
+      <c r="R6">
+        <v>4.4047899246200002</v>
+      </c>
+      <c r="S6">
+        <v>7.3223140239699998</v>
+      </c>
+      <c r="T6">
+        <v>5.3896739482899996</v>
+      </c>
+      <c r="U6">
+        <v>5.2460770607000002</v>
+      </c>
+      <c r="V6">
+        <v>5.7719390392300003</v>
+      </c>
+      <c r="W6">
+        <v>10.904332160899999</v>
+      </c>
+      <c r="X6">
+        <v>7.9445929527299999</v>
+      </c>
+      <c r="Y6">
+        <v>7.9317770004300003</v>
+      </c>
+      <c r="Z6">
+        <v>6.2514350414299997</v>
+      </c>
+      <c r="AA6">
+        <v>7.2638380527499997</v>
+      </c>
+      <c r="AB6">
+        <v>5.5871918201400002</v>
+      </c>
+      <c r="AC6">
+        <v>7.02986216545</v>
+      </c>
+      <c r="AD6">
+        <v>6.0051870346099996</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:30">
       <c r="A7" s="1">
         <v>4.4747250080100001</v>
       </c>
@@ -716,8 +1132,65 @@
       <c r="J7">
         <v>8.7818090915700004</v>
       </c>
+      <c r="K7">
+        <v>6.3250169753999996</v>
+      </c>
+      <c r="L7">
+        <v>5.3025619983699999</v>
+      </c>
+      <c r="M7">
+        <v>8.6651480197899993</v>
+      </c>
+      <c r="N7">
+        <v>5.4503090381600003</v>
+      </c>
+      <c r="O7">
+        <v>10.592983007400001</v>
+      </c>
+      <c r="P7">
+        <v>5.8459730148300002</v>
+      </c>
+      <c r="Q7">
+        <v>9.1784570217100008</v>
+      </c>
+      <c r="R7">
+        <v>4.9771451950100003</v>
+      </c>
+      <c r="S7">
+        <v>12.4114000797</v>
+      </c>
+      <c r="T7">
+        <v>4.9677929878200002</v>
+      </c>
+      <c r="U7">
+        <v>5.05774402618</v>
+      </c>
+      <c r="V7">
+        <v>3.21835398674</v>
+      </c>
+      <c r="W7">
+        <v>7.5053038597099997</v>
+      </c>
+      <c r="X7">
+        <v>8.2181968688999998</v>
+      </c>
+      <c r="Y7">
+        <v>10.7988369465</v>
+      </c>
+      <c r="Z7">
+        <v>4.4362788200400001</v>
+      </c>
+      <c r="AA7">
+        <v>10.408262968100001</v>
+      </c>
+      <c r="AC7">
+        <v>4.93013381958</v>
+      </c>
+      <c r="AD7">
+        <v>6.6710109710700003</v>
+      </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:30">
       <c r="A8" s="1">
         <v>12.4645600319</v>
       </c>
@@ -748,8 +1221,68 @@
       <c r="J8">
         <v>11.5417020321</v>
       </c>
+      <c r="K8">
+        <v>10.2413270473</v>
+      </c>
+      <c r="L8">
+        <v>5.3939101695999998</v>
+      </c>
+      <c r="M8">
+        <v>9.9313330650299996</v>
+      </c>
+      <c r="N8">
+        <v>8.1953809261299995</v>
+      </c>
+      <c r="O8">
+        <v>3.57823204994</v>
+      </c>
+      <c r="P8">
+        <v>5.1508989334099997</v>
+      </c>
+      <c r="Q8">
+        <v>8.3822860717799994</v>
+      </c>
+      <c r="R8">
+        <v>6.6645059585600004</v>
+      </c>
+      <c r="S8">
+        <v>13.1715459824</v>
+      </c>
+      <c r="T8">
+        <v>7.1846630573299999</v>
+      </c>
+      <c r="U8">
+        <v>8.9229450225800004</v>
+      </c>
+      <c r="V8">
+        <v>1.00109982491</v>
+      </c>
+      <c r="W8">
+        <v>10.5278830528</v>
+      </c>
+      <c r="X8">
+        <v>6.4035041332200002</v>
+      </c>
+      <c r="Y8">
+        <v>11.249122142799999</v>
+      </c>
+      <c r="Z8">
+        <v>9.7789721488999994</v>
+      </c>
+      <c r="AA8">
+        <v>10.5597448349</v>
+      </c>
+      <c r="AB8">
+        <v>5.7386569976799997</v>
+      </c>
+      <c r="AC8">
+        <v>11.597808837900001</v>
+      </c>
+      <c r="AD8">
+        <v>3.8952839374499999</v>
+      </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:30">
       <c r="A9" s="1">
         <v>9.3359701633499999</v>
       </c>
@@ -780,8 +1313,65 @@
       <c r="J9">
         <v>10.6595420837</v>
       </c>
+      <c r="K9">
+        <v>10.1031570435</v>
+      </c>
+      <c r="L9">
+        <v>5.7299258708999998</v>
+      </c>
+      <c r="M9">
+        <v>8.8736460208899999</v>
+      </c>
+      <c r="N9">
+        <v>10.3466620445</v>
+      </c>
+      <c r="P9">
+        <v>6.1057620048499999</v>
+      </c>
+      <c r="Q9">
+        <v>5.2762200832400001</v>
+      </c>
+      <c r="R9">
+        <v>3.7432990074200001</v>
+      </c>
+      <c r="S9">
+        <v>3.8702540397599998</v>
+      </c>
+      <c r="T9">
+        <v>4.7517189979600003</v>
+      </c>
+      <c r="U9">
+        <v>9.3388240337399999</v>
+      </c>
+      <c r="V9">
+        <v>6.98614907265</v>
+      </c>
+      <c r="W9">
+        <v>12.2675960064</v>
+      </c>
+      <c r="X9">
+        <v>4.5814630985299996</v>
+      </c>
+      <c r="Y9">
+        <v>9.5830719471000005</v>
+      </c>
+      <c r="Z9">
+        <v>5.6728358268700001</v>
+      </c>
+      <c r="AA9">
+        <v>3.84699296951</v>
+      </c>
+      <c r="AB9">
+        <v>4.3758251667000003</v>
+      </c>
+      <c r="AC9">
+        <v>8.4844601154300001</v>
+      </c>
+      <c r="AD9">
+        <v>5.0193800926199996</v>
+      </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:30">
       <c r="A10" s="1">
         <v>7.8239161968199999</v>
       </c>
@@ -812,8 +1402,68 @@
       <c r="J10">
         <v>6.3472139835399997</v>
       </c>
+      <c r="K10">
+        <v>5.8762609958600001</v>
+      </c>
+      <c r="L10">
+        <v>4.2589738369000001</v>
+      </c>
+      <c r="M10">
+        <v>8.0787611007700004</v>
+      </c>
+      <c r="N10">
+        <v>5.1648728847500003</v>
+      </c>
+      <c r="O10">
+        <v>7.98420500755</v>
+      </c>
+      <c r="P10">
+        <v>3.3259749412500001</v>
+      </c>
+      <c r="Q10">
+        <v>6.9140679836299999</v>
+      </c>
+      <c r="R10">
+        <v>4.2976059913600002</v>
+      </c>
+      <c r="S10">
+        <v>6.6214289665199999</v>
+      </c>
+      <c r="T10">
+        <v>6.1448638439199996</v>
+      </c>
+      <c r="U10">
+        <v>4.7924590110800001</v>
+      </c>
+      <c r="V10">
+        <v>5.1476149559</v>
+      </c>
+      <c r="W10">
+        <v>6.4004659652699996</v>
+      </c>
+      <c r="X10">
+        <v>4.2170639038099997</v>
+      </c>
+      <c r="Y10">
+        <v>10.0647728443</v>
+      </c>
+      <c r="Z10">
+        <v>3.6837229728700001</v>
+      </c>
+      <c r="AA10">
+        <v>8.5347650051099997</v>
+      </c>
+      <c r="AB10">
+        <v>6.4672141075100003</v>
+      </c>
+      <c r="AC10">
+        <v>7.97739291191</v>
+      </c>
+      <c r="AD10">
+        <v>6.90769219398</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:30">
       <c r="A11" s="1">
         <v>7.6263120174400001</v>
       </c>
@@ -844,8 +1494,68 @@
       <c r="J11">
         <v>9.6616528034200009</v>
       </c>
+      <c r="K11">
+        <v>6.3012020587900004</v>
+      </c>
+      <c r="L11">
+        <v>4.6434559822099999</v>
+      </c>
+      <c r="M11">
+        <v>6.2965490818000003</v>
+      </c>
+      <c r="N11">
+        <v>5.54586100578</v>
+      </c>
+      <c r="O11">
+        <v>8.5654850006099998</v>
+      </c>
+      <c r="P11">
+        <v>5.1141159534499998</v>
+      </c>
+      <c r="Q11">
+        <v>8.3117270469700006</v>
+      </c>
+      <c r="R11">
+        <v>4.6779561042799997</v>
+      </c>
+      <c r="S11">
+        <v>8.5863049030299994</v>
+      </c>
+      <c r="T11">
+        <v>4.0404109954800003</v>
+      </c>
+      <c r="U11">
+        <v>9.9192130565600003</v>
+      </c>
+      <c r="V11">
+        <v>3.4940888881699999</v>
+      </c>
+      <c r="W11">
+        <v>5.2674508094799997</v>
+      </c>
+      <c r="X11">
+        <v>4.0007019042999996</v>
+      </c>
+      <c r="Y11">
+        <v>7.3224859237700004</v>
+      </c>
+      <c r="Z11">
+        <v>8.7609698772400009</v>
+      </c>
+      <c r="AA11">
+        <v>5.28270697594</v>
+      </c>
+      <c r="AB11">
+        <v>7.2294220924400001</v>
+      </c>
+      <c r="AC11">
+        <v>6.0120949745200001</v>
+      </c>
+      <c r="AD11">
+        <v>4.2758450508100001</v>
+      </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:30">
       <c r="A12" s="1">
         <v>5.3256530761700001</v>
       </c>
@@ -876,8 +1586,68 @@
       <c r="J12">
         <v>7.7094130516100003</v>
       </c>
+      <c r="K12">
+        <v>3.7189438343000001</v>
+      </c>
+      <c r="L12">
+        <v>4.72835707664</v>
+      </c>
+      <c r="M12">
+        <v>9.67109894753</v>
+      </c>
+      <c r="N12">
+        <v>4.9142580032299996</v>
+      </c>
+      <c r="O12">
+        <v>7.4456100463899997</v>
+      </c>
+      <c r="P12">
+        <v>4.6003060340899999</v>
+      </c>
+      <c r="Q12">
+        <v>5.5972909927399996</v>
+      </c>
+      <c r="R12">
+        <v>6.55265283585</v>
+      </c>
+      <c r="S12">
+        <v>13.1080429554</v>
+      </c>
+      <c r="T12">
+        <v>4.4572448730499996</v>
+      </c>
+      <c r="U12">
+        <v>5.01047706604</v>
+      </c>
+      <c r="V12">
+        <v>6.0342168807999998</v>
+      </c>
+      <c r="W12">
+        <v>7.02970814705</v>
+      </c>
+      <c r="X12">
+        <v>3.7347660064700001</v>
+      </c>
+      <c r="Y12">
+        <v>6.6934459209400003</v>
+      </c>
+      <c r="Z12">
+        <v>14.339079141599999</v>
+      </c>
+      <c r="AA12">
+        <v>3.7221269607499998</v>
+      </c>
+      <c r="AB12">
+        <v>9.0825469493900002</v>
+      </c>
+      <c r="AC12">
+        <v>7.0391118526499996</v>
+      </c>
+      <c r="AD12">
+        <v>4.9795889854400004</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:30">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>5.2500851154300001</v>
@@ -906,8 +1676,59 @@
       <c r="J13">
         <v>10.8570451736</v>
       </c>
+      <c r="K13">
+        <v>6.4695580005600002</v>
+      </c>
+      <c r="L13">
+        <v>4.23426508904</v>
+      </c>
+      <c r="N13">
+        <v>5.3501458167999996</v>
+      </c>
+      <c r="O13">
+        <v>8.23978805542</v>
+      </c>
+      <c r="P13">
+        <v>3.2667350768999999</v>
+      </c>
+      <c r="Q13">
+        <v>5.1830308437300001</v>
+      </c>
+      <c r="R13">
+        <v>5.5593280792200002</v>
+      </c>
+      <c r="U13">
+        <v>7.4760010242500003</v>
+      </c>
+      <c r="V13">
+        <v>4.44638419151</v>
+      </c>
+      <c r="W13">
+        <v>9.3283610343899994</v>
+      </c>
+      <c r="X13">
+        <v>6.6491639614100002</v>
+      </c>
+      <c r="Y13">
+        <v>9.6735458374000007</v>
+      </c>
+      <c r="Z13">
+        <v>5.3045370578800002</v>
+      </c>
+      <c r="AA13">
+        <v>7.3936660289800002</v>
+      </c>
+      <c r="AB13">
+        <v>5.9082698821999999</v>
+      </c>
+      <c r="AC13">
+        <v>4.87900710106</v>
+      </c>
+      <c r="AD13">
+        <v>3.8953309059099999</v>
+      </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:30">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>3.76313996315</v>
@@ -936,8 +1757,53 @@
       <c r="J14">
         <v>8.14380502701</v>
       </c>
+      <c r="K14">
+        <v>7.5297110080699996</v>
+      </c>
+      <c r="L14">
+        <v>7.3666648864699997</v>
+      </c>
+      <c r="O14">
+        <v>10.974452018699999</v>
+      </c>
+      <c r="P14">
+        <v>8.5025880336800004</v>
+      </c>
+      <c r="Q14">
+        <v>8.2070469856300008</v>
+      </c>
+      <c r="R14">
+        <v>1.38490891457</v>
+      </c>
+      <c r="U14">
+        <v>9.93773794174</v>
+      </c>
+      <c r="V14">
+        <v>4.88699293137</v>
+      </c>
+      <c r="W14">
+        <v>4.4889490604400004</v>
+      </c>
+      <c r="Y14">
+        <v>6.0759251117700002</v>
+      </c>
+      <c r="Z14">
+        <v>4.2473258972199996</v>
+      </c>
+      <c r="AA14">
+        <v>9.4791910648299993</v>
+      </c>
+      <c r="AB14">
+        <v>4.3444430828099998</v>
+      </c>
+      <c r="AC14">
+        <v>6.9192278385200003</v>
+      </c>
+      <c r="AD14">
+        <v>4.2665131092099999</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:30">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>6.6069509983100003</v>
@@ -962,8 +1828,44 @@
       <c r="J15">
         <v>10.450729847</v>
       </c>
+      <c r="K15">
+        <v>7.8496789932300004</v>
+      </c>
+      <c r="O15">
+        <v>6.43407297134</v>
+      </c>
+      <c r="P15">
+        <v>9.5445101261099996</v>
+      </c>
+      <c r="Q15">
+        <v>5.9570248127000003</v>
+      </c>
+      <c r="U15">
+        <v>7.2874939441700004</v>
+      </c>
+      <c r="V15">
+        <v>6.8531439304399999</v>
+      </c>
+      <c r="W15">
+        <v>8.1330411434199998</v>
+      </c>
+      <c r="Y15">
+        <v>7.8063530921900002</v>
+      </c>
+      <c r="AA15">
+        <v>7.1805460452999998</v>
+      </c>
+      <c r="AB15">
+        <v>7.0192379951500001</v>
+      </c>
+      <c r="AC15">
+        <v>7.8132729530300002</v>
+      </c>
+      <c r="AD15">
+        <v>5.16345191002</v>
+      </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:30">
       <c r="G16">
         <v>12.3399178982</v>
       </c>
@@ -973,14 +1875,32 @@
       <c r="J16">
         <v>11.102599143999999</v>
       </c>
+      <c r="K16">
+        <v>5.7738459110299996</v>
+      </c>
+      <c r="Q16">
+        <v>6.7515971660599998</v>
+      </c>
+      <c r="U16">
+        <v>11.2311151028</v>
+      </c>
+      <c r="V16">
+        <v>5.4174311161000004</v>
+      </c>
+      <c r="AA16">
+        <v>10.5219619274</v>
+      </c>
+      <c r="AB16">
+        <v>4.27748990059</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1">
+    <row r="17" spans="1:30" s="4" customFormat="1">
       <c r="A17" s="4">
         <f>AVERAGE(A2:A16)</f>
         <v>7.1603120023554538</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" ref="B17:J17" si="0">AVERAGE(B2:B16)</f>
+        <f t="shared" ref="B17:AD17" si="0">AVERAGE(B2:B16)</f>
         <v>7.0463251150553834</v>
       </c>
       <c r="C17" s="4">
@@ -1015,8 +1935,88 @@
         <f t="shared" si="0"/>
         <v>9.7599684079486675</v>
       </c>
+      <c r="K17" s="4">
+        <f t="shared" si="0"/>
+        <v>7.3288404782579999</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0046709867630774</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="0"/>
+        <v>8.9158502275254534</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="0"/>
+        <v>6.065459986524167</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="0"/>
+        <v>8.4649856640676902</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6283782262069231</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="0"/>
+        <v>6.7990440686546663</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4654203745030774</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="0"/>
+        <v>9.2014751867818187</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="0"/>
+        <v>6.2519239425649999</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="0"/>
+        <v>7.396290747326665</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4859182834626674</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="0"/>
+        <v>8.2044283492150001</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5247805335309099</v>
+      </c>
+      <c r="Y17" s="4">
+        <f t="shared" si="0"/>
+        <v>8.1672589778899987</v>
+      </c>
+      <c r="Z17" s="4">
+        <f t="shared" si="0"/>
+        <v>6.6970565716424986</v>
+      </c>
+      <c r="AA17" s="4">
+        <f t="shared" si="0"/>
+        <v>7.4737285772940014</v>
+      </c>
+      <c r="AB17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.9954125199964281</v>
+      </c>
+      <c r="AC17" s="4">
+        <f t="shared" si="0"/>
+        <v>7.1297611679349986</v>
+      </c>
+      <c r="AD17" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3322523491721423</v>
+      </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:30">
       <c r="A18">
         <f>MEDIAN(A2:A16)</f>
         <v>7.6263120174400001</v>
@@ -1058,7 +2058,7 @@
         <v>9.6616528034200009</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:30">
       <c r="A26" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
save the rough extimation excel file
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37580" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37440" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -674,9 +674,7 @@
       <c r="D2" s="1">
         <v>7.8090708255800001</v>
       </c>
-      <c r="E2" s="1">
-        <v>22.310221910500001</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1">
         <v>9.3382551670100007</v>
       </c>
@@ -1913,7 +1911,7 @@
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>9.859899795976153</v>
+        <v>8.8223729530991655</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="0"/>
@@ -2035,7 +2033,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>7.2980821132699996</v>
+        <v>7.0182945728299995</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>

</xml_diff>